<commit_message>
Update from Joost's version [05/06]
</commit_message>
<xml_diff>
--- a/scenario/remon_raw_scenario/AC Type 2.xlsx
+++ b/scenario/remon_raw_scenario/AC Type 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Git 2\queries\remon raw scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\BlueSky_Joost\scenario\remon_raw_scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419C006C-5FDC-479D-B7B3-EF9B8F86C084}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E23DC-617C-48B1-AC50-A3D3D0979584}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="1305" windowWidth="10695" windowHeight="13950" xr2:uid="{387ECC03-4236-429D-882A-E101A289F3C1}"/>
+    <workbookView xWindow="7185" yWindow="1125" windowWidth="21465" windowHeight="13785" xr2:uid="{387ECC03-4236-429D-882A-E101A289F3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,74 +455,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -539,10 +471,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFF00"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -834,10 +766,13 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>